<commit_message>
Operation of send and receive data to/from MQTT work fine
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4643" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20867" uniqueCount="208">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -400,6 +400,321 @@
   </si>
   <si>
     <t xml:space="preserve">123 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can dispatch &lt;value&gt; volumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can dispatch &lt;value&gt; liters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
   </si>
 </sst>
 </file>
@@ -2462,6 +2777,108 @@
         <v>126</v>
       </c>
     </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added Pop up alerting problem on connection with network or broker MQTT and credential invalid. Also I added function to parse response of credential and storage liters available.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20867" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25829" uniqueCount="239">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -715,6 +715,127 @@
   <si>
     <t xml:space="preserve">Invalid credencial, 
 try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credencial, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credential, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem with MQTT
+server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credential, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem with MQTT
+server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credential, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem with MQTT
+server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credential, 
+try again please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn't connect to network,
+try again please.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem with MQTT
+server</t>
   </si>
 </sst>
 </file>
@@ -2791,7 +2912,7 @@
         <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34">
@@ -2877,6 +2998,57 @@
       </c>
       <c r="F38" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>209</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>211</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Send amount of liters that I would like to dispatch and parser of response
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25829" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27511" uniqueCount="246">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -836,6 +836,31 @@
   <si>
     <t xml:space="preserve">Problem with MQTT
 server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can´t dispense this amount
+ of fuel, please enter less liters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can´t dispense this amount
+ of fuel, please enter less liters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can´t dispense this amount
+ of fuel, please enter less liters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can´t dispense this amount
+ of fuel, please enter less liters</t>
   </si>
 </sst>
 </file>
@@ -2113,9 +2138,13 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
       <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -2912,7 +2941,7 @@
         <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34">
@@ -3031,7 +3060,7 @@
         <v>42</v>
       </c>
       <c r="F40" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41">
@@ -3048,9 +3077,44 @@
         <v>42</v>
       </c>
       <c r="F41" t="s">
-        <v>238</v>
-      </c>
-    </row>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>240</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added NFC functionality, also I created screen to set up MQTT parameters
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27511" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43005" uniqueCount="314">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -861,6 +861,254 @@
   <si>
     <t xml:space="preserve">You can´t dispense this amount
  of fuel, please enter less liters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingrese </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem with service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome
+Thank you for choosing us
+Control GAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome
+Thank you for choosing us
+Control GAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome and
+Thank you for choosing us
+Control GAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version MQTT 3.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QoS type 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QoS type 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QoS type 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client ID: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publish topic: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QoS type 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep alive
+ (Second)</t>
   </si>
 </sst>
 </file>
@@ -2618,15 +2866,15 @@
         <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
@@ -2635,15 +2883,15 @@
         <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
         <v>41</v>
@@ -2652,12 +2900,12 @@
         <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
         <v>63</v>
@@ -2669,12 +2917,12 @@
         <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
@@ -2686,15 +2934,15 @@
         <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
@@ -2703,32 +2951,32 @@
         <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
         <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>41</v>
@@ -2737,32 +2985,32 @@
         <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
         <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
@@ -2771,15 +3019,15 @@
         <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
         <v>41</v>
@@ -2788,15 +3036,15 @@
         <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
         <v>41</v>
@@ -2805,15 +3053,15 @@
         <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
         <v>41</v>
@@ -2822,15 +3070,15 @@
         <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s">
         <v>41</v>
@@ -2839,49 +3087,49 @@
         <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
         <v>42</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
         <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
         <v>76</v>
@@ -2890,46 +3138,46 @@
         <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
         <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="C33" t="s">
         <v>63</v>
@@ -2941,12 +3189,12 @@
         <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>129</v>
+        <v>194</v>
       </c>
       <c r="C34" t="s">
         <v>63</v>
@@ -2958,80 +3206,80 @@
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C35" t="s">
         <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
         <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>116</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C36" t="s">
         <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
         <v>42</v>
       </c>
       <c r="F36" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
         <v>63</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
         <v>42</v>
       </c>
       <c r="F37" t="s">
-        <v>200</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
         <v>63</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s">
         <v>42</v>
       </c>
       <c r="F38" t="s">
-        <v>62</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C39" t="s">
         <v>63</v>
@@ -3043,15 +3291,15 @@
         <v>42</v>
       </c>
       <c r="F39" t="s">
-        <v>130</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>209</v>
+        <v>239</v>
       </c>
       <c r="C40" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
         <v>41</v>
@@ -3060,12 +3308,12 @@
         <v>42</v>
       </c>
       <c r="F40" t="s">
-        <v>210</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="C41" t="s">
         <v>63</v>
@@ -3077,15 +3325,15 @@
         <v>42</v>
       </c>
       <c r="F41" t="s">
-        <v>229</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
         <v>41</v>
@@ -3094,12 +3342,12 @@
         <v>42</v>
       </c>
       <c r="F42" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C43" t="s">
         <v>63</v>
@@ -3111,10 +3359,264 @@
         <v>42</v>
       </c>
       <c r="F43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>255</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>257</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>259</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>263</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="44"/>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>264</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F50" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>268</v>
+      </c>
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" t="s">
+        <v>76</v>
+      </c>
+      <c r="E53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>269</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>271</v>
+      </c>
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F55" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>272</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>76</v>
+      </c>
+      <c r="E56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F56" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>274</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>275</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" t="s">
+        <v>276</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added interaction with task NFC and NFC screen, timer of screen implemented.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43005" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44171" uniqueCount="323">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1109,6 +1109,33 @@
   <si>
     <t xml:space="preserve">Keep alive
  (Second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest waiting time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Card read was: </t>
   </si>
 </sst>
 </file>
@@ -2352,7 +2379,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>93</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -3347,10 +3376,10 @@
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C43" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
         <v>41</v>
@@ -3359,29 +3388,29 @@
         <v>42</v>
       </c>
       <c r="F43" t="s">
-        <v>116</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
         <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
@@ -3393,12 +3422,12 @@
         <v>42</v>
       </c>
       <c r="F45" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C46" t="s">
         <v>38</v>
@@ -3410,12 +3439,12 @@
         <v>42</v>
       </c>
       <c r="F46" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -3427,15 +3456,15 @@
         <v>42</v>
       </c>
       <c r="F47" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
         <v>76</v>
@@ -3444,15 +3473,15 @@
         <v>42</v>
       </c>
       <c r="F48" t="s">
-        <v>262</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="D49" t="s">
         <v>76</v>
@@ -3461,15 +3490,15 @@
         <v>42</v>
       </c>
       <c r="F49" t="s">
-        <v>87</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C50" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D50" t="s">
         <v>76</v>
@@ -3478,15 +3507,15 @@
         <v>42</v>
       </c>
       <c r="F50" t="s">
-        <v>265</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="D51" t="s">
         <v>76</v>
@@ -3495,15 +3524,15 @@
         <v>42</v>
       </c>
       <c r="F51" t="s">
-        <v>87</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D52" t="s">
         <v>76</v>
@@ -3512,32 +3541,32 @@
         <v>42</v>
       </c>
       <c r="F52" t="s">
-        <v>265</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="D53" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E53" t="s">
         <v>42</v>
       </c>
       <c r="F53" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C54" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="D54" t="s">
         <v>41</v>
@@ -3546,46 +3575,46 @@
         <v>42</v>
       </c>
       <c r="F54" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E55" t="s">
         <v>42</v>
       </c>
       <c r="F55" t="s">
-        <v>87</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C56" t="s">
         <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E56" t="s">
         <v>42</v>
       </c>
       <c r="F56" t="s">
-        <v>313</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C57" t="s">
         <v>38</v>
@@ -3597,26 +3626,95 @@
         <v>42</v>
       </c>
       <c r="F57" t="s">
-        <v>130</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="C58" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>315</v>
+      </c>
+      <c r="C59" t="s">
         <v>38</v>
       </c>
-      <c r="D58" t="s">
-        <v>41</v>
-      </c>
-      <c r="E58" t="s">
-        <v>42</v>
-      </c>
-      <c r="F58" t="s">
-        <v>276</v>
-      </c>
-    </row>
+      <c r="D59" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>316</v>
+      </c>
+      <c r="C60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" t="s">
+        <v>42</v>
+      </c>
+      <c r="F60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>319</v>
+      </c>
+      <c r="C61" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" t="s">
+        <v>42</v>
+      </c>
+      <c r="F61" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>321</v>
+      </c>
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="63"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Solve problem with configuration on MQTT parameters and send credention card to broker MQTT
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44171" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44564" uniqueCount="323">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2380,7 +2380,7 @@
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">

</xml_diff>

<commit_message>
Get credential of card nfc or manual done as well as send credential to broker for MQTT and parse renponse. Was added task to drive controller pump.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44564" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44957" uniqueCount="325">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1136,6 +1136,12 @@
   </si>
   <si>
     <t xml:space="preserve">Card read was: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
   </si>
 </sst>
 </file>
@@ -3631,44 +3637,44 @@
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E58" t="s">
         <v>42</v>
       </c>
       <c r="F58" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C59" t="s">
         <v>38</v>
       </c>
       <c r="D59" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E59" t="s">
         <v>42</v>
       </c>
       <c r="F59" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C60" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D60" t="s">
         <v>76</v>
@@ -3677,12 +3683,12 @@
         <v>42</v>
       </c>
       <c r="F60" t="s">
-        <v>62</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C61" t="s">
         <v>63</v>
@@ -3694,15 +3700,15 @@
         <v>42</v>
       </c>
       <c r="F61" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C62" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="D62" t="s">
         <v>76</v>
@@ -3711,7 +3717,7 @@
         <v>42</v>
       </c>
       <c r="F62" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63"/>

</xml_diff>

<commit_message>
UI of operation pump with builder and parser of main request/response message from/to pump controller done.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44957" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45392" uniqueCount="338">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1142,6 +1142,45 @@
   </si>
   <si>
     <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPACHE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANCEL SALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAY SALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liters filled: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operation: &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -3720,7 +3759,125 @@
         <v>324</v>
       </c>
     </row>
-    <row r="63"/>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>325</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>327</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>329</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>41</v>
+      </c>
+      <c r="E65" t="s">
+        <v>42</v>
+      </c>
+      <c r="F65" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>331</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>333</v>
+      </c>
+      <c r="C67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D67" t="s">
+        <v>41</v>
+      </c>
+      <c r="E67" t="s">
+        <v>42</v>
+      </c>
+      <c r="F67" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>335</v>
+      </c>
+      <c r="C68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" t="s">
+        <v>42</v>
+      </c>
+      <c r="F68" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>336</v>
+      </c>
+      <c r="C69" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" t="s">
+        <v>41</v>
+      </c>
+      <c r="E69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F69" t="s">
+        <v>337</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added function on GUI to dispatch and stop pump
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45392" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47687" uniqueCount="350">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1181,6 +1181,42 @@
   </si>
   <si>
     <t xml:space="preserve">Operation: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pump selected is: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPATCH</t>
   </si>
 </sst>
 </file>
@@ -3773,7 +3809,7 @@
         <v>42</v>
       </c>
       <c r="F63" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
     </row>
     <row r="64">
@@ -3795,7 +3831,7 @@
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C65" t="s">
         <v>38</v>
@@ -3807,15 +3843,15 @@
         <v>42</v>
       </c>
       <c r="F65" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C66" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
         <v>41</v>
@@ -3824,46 +3860,46 @@
         <v>42</v>
       </c>
       <c r="F66" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C67" t="s">
         <v>63</v>
       </c>
       <c r="D67" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="E67" t="s">
         <v>42</v>
       </c>
       <c r="F67" t="s">
-        <v>334</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C68" t="s">
         <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E68" t="s">
         <v>42</v>
       </c>
       <c r="F68" t="s">
-        <v>62</v>
+        <v>339</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C69" t="s">
         <v>63</v>
@@ -3875,7 +3911,92 @@
         <v>42</v>
       </c>
       <c r="F69" t="s">
-        <v>337</v>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>342</v>
+      </c>
+      <c r="C70" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" t="s">
+        <v>41</v>
+      </c>
+      <c r="E70" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>344</v>
+      </c>
+      <c r="C71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" t="s">
+        <v>42</v>
+      </c>
+      <c r="F71" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>346</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" t="s">
+        <v>42</v>
+      </c>
+      <c r="F72" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>348</v>
+      </c>
+      <c r="C73" t="s">
+        <v>63</v>
+      </c>
+      <c r="D73" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" t="s">
+        <v>42</v>
+      </c>
+      <c r="F73" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>329</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" t="s">
+        <v>42</v>
+      </c>
+      <c r="F74" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setup stack size FreeRTOS from 15KB to 25KB and fishish updater liters filler on GUI
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47687" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48165" uniqueCount="352">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1217,6 +1217,12 @@
   </si>
   <si>
     <t xml:space="preserve">DISPATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
   </si>
 </sst>
 </file>
@@ -2458,7 +2464,9 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
       <c r="H4"/>
       <c r="I4" t="s">
         <v>99</v>
@@ -3999,6 +4007,40 @@
         <v>330</v>
       </c>
     </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>350</v>
+      </c>
+      <c r="C75" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" t="s">
+        <v>76</v>
+      </c>
+      <c r="E75" t="s">
+        <v>42</v>
+      </c>
+      <c r="F75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>351</v>
+      </c>
+      <c r="C76" t="s">
+        <v>63</v>
+      </c>
+      <c r="D76" t="s">
+        <v>41</v>
+      </c>
+      <c r="E76" t="s">
+        <v>42</v>
+      </c>
+      <c r="F76" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Sent sale finalization and receive response done.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48165" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48643" uniqueCount="353">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1223,6 +1223,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subscribe topic: </t>
   </si>
 </sst>
 </file>
@@ -3613,7 +3616,7 @@
         <v>42</v>
       </c>
       <c r="F51" t="s">
-        <v>265</v>
+        <v>352</v>
       </c>
     </row>
     <row r="52">

</xml_diff>